<commit_message>
:wrench:fix: Removed IOU part, training Part - tested Fine.
</commit_message>
<xml_diff>
--- a/weights/trained_iwpodnet.xlsx
+++ b/weights/trained_iwpodnet.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>24.10939788818359</v>
+        <v>42.50841522216797</v>
       </c>
       <c r="C2" t="n">
         <v>0.001000000047497451</v>
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>14.67454433441162</v>
+        <v>30.18067932128906</v>
       </c>
       <c r="C3" t="n">
         <v>0.001000000047497451</v>
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10.99068927764893</v>
+        <v>20.48553085327148</v>
       </c>
       <c r="C4" t="n">
         <v>0.001000000047497451</v>
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7.399983882904053</v>
+        <v>16.6971492767334</v>
       </c>
       <c r="C5" t="n">
         <v>0.000199999994947575</v>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8.507196426391602</v>
+        <v>14.62571907043457</v>
       </c>
       <c r="C6" t="n">
         <v>0.000199999994947575</v>
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>8.375302314758301</v>
+        <v>13.11354351043701</v>
       </c>
       <c r="C7" t="n">
         <v>0.000199999994947575</v>
@@ -516,7 +516,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>8.673244476318359</v>
+        <v>12.80695533752441</v>
       </c>
       <c r="C8" t="n">
         <v>3.999999898951501e-05</v>
@@ -527,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>7.50892448425293</v>
+        <v>12.56159400939941</v>
       </c>
       <c r="C9" t="n">
         <v>3.999999898951501e-05</v>
@@ -538,7 +538,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>7.2325119972229</v>
+        <v>13.35915660858154</v>
       </c>
       <c r="C10" t="n">
         <v>3.999999898951501e-05</v>
@@ -549,7 +549,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>5.214747905731201</v>
+        <v>13.80314922332764</v>
       </c>
       <c r="C11" t="n">
         <v>3.999999898951501e-05</v>

</xml_diff>